<commit_message>
update python link in excel examples
</commit_message>
<xml_diff>
--- a/helper/cloud config file examples/config2.xlsx
+++ b/helper/cloud config file examples/config2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joa_n\Noorjax Dropbox\Joaquin Guzman\Ferag Tests\01 - Models\AutoSorting 0.3.4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Noorjax Dropbox\felipe haro\00 - current\ferag\Ferag - Generic Conveyor System\07 - AutoSorting Library\sorting_conveyors\helper\cloud config file examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{655A12D1-FEAD-4CAB-A7F6-441E10D0D177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7B2B97-EEE4-4EBB-A2D2-12FF87B587E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="839" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="839" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="License" sheetId="12" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="202">
   <si>
     <t>id</t>
   </si>
@@ -642,19 +642,16 @@
     <t>pythonPath</t>
   </si>
   <si>
-    <t>C:\Users\Joa_n\anaconda3\python.exe</t>
-  </si>
-  <si>
     <t>Only used to show the conveyor drawing in the conveyors config tab</t>
   </si>
   <si>
-    <t>C:\Users\felip\anaconda3\python.exe</t>
-  </si>
-  <si>
     <t>Insert token below</t>
   </si>
   <si>
     <t>ok96u4mqb9c0HRtjp1GKEZviFKF9QpkKDDWgcPyo05DrTrvd658yMELvXI2KF9aO</t>
+  </si>
+  <si>
+    <t>C:\Users\username\anaconda3\python.exe</t>
   </si>
 </sst>
 </file>
@@ -662,7 +659,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -716,7 +713,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1005,19 +1002,19 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="67.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -1028,20 +1025,20 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C405D84C-1CA7-49B6-B9D3-19C2E49B9A7B}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1052,7 +1049,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1063,20 +1060,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>197</v>
       </c>
       <c r="B3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" t="s">
         <v>198</v>
-      </c>
-      <c r="C3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -1094,25 +1086,25 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="16.5546875" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.54296875" customWidth="1"/>
+    <col min="10" max="10" width="15.90625" customWidth="1"/>
+    <col min="11" max="11" width="16.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1147,7 +1139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>169</v>
       </c>
@@ -1182,7 +1174,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>170</v>
       </c>
@@ -1217,7 +1209,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>171</v>
       </c>
@@ -1252,7 +1244,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>172</v>
       </c>
@@ -1287,7 +1279,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>173</v>
       </c>
@@ -1322,7 +1314,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>174</v>
       </c>
@@ -1357,7 +1349,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>187</v>
       </c>
@@ -1392,7 +1384,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E13" s="1"/>
     </row>
   </sheetData>
@@ -1426,14 +1418,14 @@
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="15.21875" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="1" max="2" width="15.1796875" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1450,7 +1442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>170</v>
       </c>
@@ -1467,7 +1459,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>173</v>
       </c>
@@ -1484,7 +1476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>190</v>
       </c>
@@ -1501,7 +1493,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>191</v>
       </c>
@@ -1544,18 +1536,18 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1578,7 +1570,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>180</v>
       </c>
@@ -1601,7 +1593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -1650,18 +1642,18 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.90625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1706,13 +1698,13 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1720,7 +1712,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>167</v>
       </c>
@@ -1728,7 +1720,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>168</v>
       </c>
@@ -1736,7 +1728,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -1759,692 +1751,692 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>53</v>
       </c>

</xml_diff>